<commit_message>
making test.xlsx to show grace
</commit_message>
<xml_diff>
--- a/Data/leachate.xlsx
+++ b/Data/leachate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredflater/Desktop/Flater_soilColumnAnalysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8F49D5-A37F-E74F-A71E-8547F392C7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330221B5-7EA7-3348-889C-23E5229168BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
   </bookViews>
@@ -1171,7 +1171,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2483,7 +2483,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>